<commit_message>
Selenium_To Do List_Test Case_v1.1_테스트 결과_20240309.xlsx 수정
</commit_message>
<xml_diff>
--- a/Selenium_To Do List_Test Case_v1.1_테스트 결과_20240309.xlsx
+++ b/Selenium_To Do List_Test Case_v1.1_테스트 결과_20240309.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhsdb\Desktop\포트폴리오\TC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706F1111-615E-468F-9118-383E3B080665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D866D5A-1148-4E0D-B1D8-7E29829BAE69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{6C457D58-EB79-43DF-AE70-B6D33573AE26}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{6C457D58-EB79-43DF-AE70-B6D33573AE26}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Summary Report" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="309">
   <si>
     <t>Depth1</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1354,6 +1354,19 @@
     <t>1. 현재 화면 유지하며, alert 표시
 ("내용 or 날짜를 입력하세요.")
 2. alert 사라지며 메인 화면 표시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HLD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>20240311
+2. test ti 포함하는지 mcoah.js로 작성하여 확인</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2676,7 +2689,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5E7BCF-AC80-4316-AB9E-EE8DE2654802}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="H10" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4394,7 +4409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AB6893F-AFA8-447D-8538-2948A52B3B2E}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -4635,8 +4650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F40B9D5A-690E-47CB-B8DA-5BED431D5F21}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4763,7 +4778,7 @@
         <v>229</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="J4" s="16"/>
       <c r="K4" s="5">
@@ -4787,9 +4802,13 @@
       <c r="H5" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="I5" s="9"/>
+      <c r="I5" s="9" t="s">
+        <v>307</v>
+      </c>
       <c r="J5" s="16"/>
-      <c r="K5" s="5"/>
+      <c r="K5" s="5" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A6" s="26"/>
@@ -4808,9 +4827,13 @@
       <c r="H6" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="I6" s="9"/>
+      <c r="I6" s="9" t="s">
+        <v>306</v>
+      </c>
       <c r="J6" s="16"/>
-      <c r="K6" s="5"/>
+      <c r="K6" s="5">
+        <v>20240311</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A7" s="26"/>
@@ -4829,9 +4852,13 @@
       <c r="H7" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="I7" s="9"/>
+      <c r="I7" s="9" t="s">
+        <v>307</v>
+      </c>
       <c r="J7" s="16"/>
-      <c r="K7" s="5"/>
+      <c r="K7" s="5" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A8" s="26"/>
@@ -4850,9 +4877,13 @@
       <c r="H8" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="I8" s="9"/>
+      <c r="I8" s="9" t="s">
+        <v>306</v>
+      </c>
       <c r="J8" s="16"/>
-      <c r="K8" s="5"/>
+      <c r="K8" s="5">
+        <v>20240311</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A9" s="26"/>
@@ -4871,9 +4902,13 @@
       <c r="H9" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="I9" s="9"/>
+      <c r="I9" s="9" t="s">
+        <v>307</v>
+      </c>
       <c r="J9" s="16"/>
-      <c r="K9" s="5"/>
+      <c r="K9" s="5" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A10" s="26"/>
@@ -4892,9 +4927,13 @@
       <c r="H10" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="I10" s="9"/>
+      <c r="I10" s="9" t="s">
+        <v>306</v>
+      </c>
       <c r="J10" s="16"/>
-      <c r="K10" s="5"/>
+      <c r="K10" s="5">
+        <v>20240311</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A11" s="26"/>
@@ -4913,9 +4952,13 @@
       <c r="H11" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="I11" s="9"/>
+      <c r="I11" s="9" t="s">
+        <v>307</v>
+      </c>
       <c r="J11" s="16"/>
-      <c r="K11" s="5"/>
+      <c r="K11" s="5" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A12" s="26"/>
@@ -4936,9 +4979,13 @@
       <c r="H12" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="I12" s="9"/>
+      <c r="I12" s="9" t="s">
+        <v>306</v>
+      </c>
       <c r="J12" s="16"/>
-      <c r="K12" s="5"/>
+      <c r="K12" s="5">
+        <v>20240311</v>
+      </c>
     </row>
     <row r="13" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A13" s="26"/>
@@ -4957,9 +5004,13 @@
       <c r="H13" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I13" s="9"/>
+      <c r="I13" s="9" t="s">
+        <v>306</v>
+      </c>
       <c r="J13" s="16"/>
-      <c r="K13" s="5"/>
+      <c r="K13" s="5">
+        <v>20240311</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A14" s="26"/>
@@ -4978,9 +5029,13 @@
       <c r="H14" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="I14" s="9"/>
+      <c r="I14" s="9" t="s">
+        <v>306</v>
+      </c>
       <c r="J14" s="16"/>
-      <c r="K14" s="5"/>
+      <c r="K14" s="5">
+        <v>20240311</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A15" s="26"/>
@@ -4999,9 +5054,13 @@
       <c r="H15" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="I15" s="9"/>
+      <c r="I15" s="9" t="s">
+        <v>306</v>
+      </c>
       <c r="J15" s="16"/>
-      <c r="K15" s="5"/>
+      <c r="K15" s="5">
+        <v>20240311</v>
+      </c>
     </row>
     <row r="16" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="A16" s="26"/>

</xml_diff>